<commit_message>
Day 2 part 2 (jesus christ)
</commit_message>
<xml_diff>
--- a/Felix/Day1/24d1p1.xlsx
+++ b/Felix/Day1/24d1p1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b58bf48a7331aef/Documents/AdventOfCode/aoc24/Felix/Day1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{20D08B3D-A5C9-4485-8111-2FC84C329C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F41174E-AEA5-489D-AD19-721E714348F3}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{20D08B3D-A5C9-4485-8111-2FC84C329C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27F51B3E-0728-4AEC-8AAF-FAEE6A9D6B00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DFDEBE1-1BA3-43B7-936B-A2F432A84558}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>